<commit_message>
All translation keywords updated
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Office\SPEA\spea-x-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0146F08B-A39A-4F39-B499-9A2639725A59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7BFB60-555A-4394-88CC-9382D00F00B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="162">
   <si>
     <t>PRIVATE SCHOOLS DATA</t>
   </si>
@@ -92,13 +92,427 @@
   </si>
   <si>
     <t>اي</t>
+  </si>
+  <si>
+    <t>Sharjah Education Map</t>
+  </si>
+  <si>
+    <t>Fees</t>
+  </si>
+  <si>
+    <t>Find Schools</t>
+  </si>
+  <si>
+    <t>Advanced Search</t>
+  </si>
+  <si>
+    <t>Clear Filters</t>
+  </si>
+  <si>
+    <t>Teacher to Student Ratio</t>
+  </si>
+  <si>
+    <t>Availability of Nursery/Preschool</t>
+  </si>
+  <si>
+    <t>Recreational Facilities</t>
+  </si>
+  <si>
+    <t>Facilities for SEND Students</t>
+  </si>
+  <si>
+    <t>Searching for schools</t>
+  </si>
+  <si>
+    <t>Schools Found</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>Visit Website</t>
+  </si>
+  <si>
+    <t>Get Directions</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>Enrollment &amp; Capacity</t>
+  </si>
+  <si>
+    <t>Facilities and Services</t>
+  </si>
+  <si>
+    <t>Special Educational Needs Capacity</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>Municipality</t>
+  </si>
+  <si>
+    <t>Average Tuition Fees (AED)</t>
+  </si>
+  <si>
+    <t>Curriculum</t>
+  </si>
+  <si>
+    <t>Student Gender</t>
+  </si>
+  <si>
+    <t>Accreditation</t>
+  </si>
+  <si>
+    <t>PISA - Average Reading Literacy Score</t>
+  </si>
+  <si>
+    <t>PISA- Average Mathematical Literacy Score</t>
+  </si>
+  <si>
+    <t>affiliated with an international school/nursery or group</t>
+  </si>
+  <si>
+    <t>Total Students Enrolled</t>
+  </si>
+  <si>
+    <t>Current Available Seats</t>
+  </si>
+  <si>
+    <t>Early Years - Nursery/ Pre-Reception</t>
+  </si>
+  <si>
+    <t>KG 1 Pre-Kindergarten/Reception</t>
+  </si>
+  <si>
+    <t>KG 2 Kindergarten/Year 1</t>
+  </si>
+  <si>
+    <t>Facilities</t>
+  </si>
+  <si>
+    <t>Swimming pools</t>
+  </si>
+  <si>
+    <t>Gyms</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Not Available</t>
+  </si>
+  <si>
+    <t>Playgrounds</t>
+  </si>
+  <si>
+    <t>Air conditioned playing Courts</t>
+  </si>
+  <si>
+    <t>Open air playing Courts</t>
+  </si>
+  <si>
+    <t>Cafeterias/Lunch Areas</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Yes, provided by the school/nursery</t>
+  </si>
+  <si>
+    <t>No provided transportation</t>
+  </si>
+  <si>
+    <t>Sports/Fitness Activities</t>
+  </si>
+  <si>
+    <t>Creative Activities</t>
+  </si>
+  <si>
+    <t>Academic and Work-Related Activities</t>
+  </si>
+  <si>
+    <t>equipped for SEND students</t>
+  </si>
+  <si>
+    <t>Special Educational Need(s) Catered To</t>
+  </si>
+  <si>
+    <t>counseling sessions for parents of SEND students</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Special Education Staff Resources</t>
+  </si>
+  <si>
+    <t>Support Services</t>
+  </si>
+  <si>
+    <t>Assistive Equipment and Facilities Provided</t>
+  </si>
+  <si>
+    <t>متوفر</t>
+  </si>
+  <si>
+    <t>غير متوفر</t>
+  </si>
+  <si>
+    <t>خريطة الشارقة التعليمية</t>
+  </si>
+  <si>
+    <t>رسوم</t>
+  </si>
+  <si>
+    <t>البحث عن المدارس</t>
+  </si>
+  <si>
+    <t>بحث متقدم</t>
+  </si>
+  <si>
+    <t>مسح الفلاتر</t>
+  </si>
+  <si>
+    <t>نسبة المعلمين إلى الطلاب</t>
+  </si>
+  <si>
+    <t>توافر الحضانة / مرحلة ما قبل المدرسة</t>
+  </si>
+  <si>
+    <t>المرافق الترفيهية</t>
+  </si>
+  <si>
+    <t>المدارس التي تم العثور عليها</t>
+  </si>
+  <si>
+    <t>غلق</t>
+  </si>
+  <si>
+    <t>زيارة الموقع</t>
+  </si>
+  <si>
+    <t>احصل على الاتجاهات</t>
+  </si>
+  <si>
+    <t>نظره عامه</t>
+  </si>
+  <si>
+    <t>التسجيل والسعة</t>
+  </si>
+  <si>
+    <t>المرافق والخدمات</t>
+  </si>
+  <si>
+    <t>القدرة الاستيعابية لذوي الاحتياجات التعليمية الخاصة</t>
+  </si>
+  <si>
+    <t>مدينة</t>
+  </si>
+  <si>
+    <t>بلدية</t>
+  </si>
+  <si>
+    <t>متوسط الرسوم الدراسية (درهم)</t>
+  </si>
+  <si>
+    <t>منهاج</t>
+  </si>
+  <si>
+    <t>AED</t>
+  </si>
+  <si>
+    <t>درهم</t>
+  </si>
+  <si>
+    <t>جنس الطالب</t>
+  </si>
+  <si>
+    <t>اعتماد</t>
+  </si>
+  <si>
+    <t>بيزا - متوسط درجة معرفة القراءة والكتابة</t>
+  </si>
+  <si>
+    <t>بيزا- متوسط درجة معرفة القراءة والكتابة الرياضية</t>
+  </si>
+  <si>
+    <t>تابعة لمدرسة / حضانة أو مجموعة دولية</t>
+  </si>
+  <si>
+    <t>مجموع الطلاب المسجلين</t>
+  </si>
+  <si>
+    <t>المقاعد المتاحة حاليا</t>
+  </si>
+  <si>
+    <t>السنوات المبكرة - الحضانة / ما قبل الاستقبال</t>
+  </si>
+  <si>
+    <t>مرافق</t>
+  </si>
+  <si>
+    <t>حمامات السباحة</t>
+  </si>
+  <si>
+    <t>الصالات الرياضيه</t>
+  </si>
+  <si>
+    <t>الملاعب</t>
+  </si>
+  <si>
+    <t>ملاعب مكيفة الهواء</t>
+  </si>
+  <si>
+    <t>ملاعب اللعب في الهواء الطلق</t>
+  </si>
+  <si>
+    <t>الكافيتريات / مناطق الغداء</t>
+  </si>
+  <si>
+    <t>النقل</t>
+  </si>
+  <si>
+    <t>نعم ، مقدمة من المدرسة / الحضانة</t>
+  </si>
+  <si>
+    <t>لا توجد وسائل نقل مقدمة</t>
+  </si>
+  <si>
+    <t>الأنشطة الرياضية / اللياقة البدنية</t>
+  </si>
+  <si>
+    <t>الأنشطة الإبداعية</t>
+  </si>
+  <si>
+    <t>الأنشطة الأكاديمية والمتعلقة بالعمل</t>
+  </si>
+  <si>
+    <t>الاحتياجات التعليمية الخاصة التي يتم تلبيتها</t>
+  </si>
+  <si>
+    <t>درجة</t>
+  </si>
+  <si>
+    <t>موارد موظفي التربية الخاصة</t>
+  </si>
+  <si>
+    <t>خدمات الدعم</t>
+  </si>
+  <si>
+    <t>المعدات والمرافق المساعدة المقدمة</t>
+  </si>
+  <si>
+    <t>سنة</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>PISA - Average Scientific Literacy Score</t>
+  </si>
+  <si>
+    <t>بيزا - متوسط درجة محو الأمية العلمية</t>
+  </si>
+  <si>
+    <t>ك جم 1 مرحلة ما قبل الروضة / الاستقبال</t>
+  </si>
+  <si>
+    <t>ك جم 2 رياض الأطفال / السنة 1</t>
+  </si>
+  <si>
+    <t>مجهزة لطلاب ارسل</t>
+  </si>
+  <si>
+    <t>جلسات إرشادية لأولياء أمور طلاب ارسل</t>
+  </si>
+  <si>
+    <t>مرافق لطلاب ارسل</t>
+  </si>
+  <si>
+    <t>Back to results</t>
+  </si>
+  <si>
+    <t>العودة إلى النتائج</t>
+  </si>
+  <si>
+    <t>Facilities &amp; Services</t>
+  </si>
+  <si>
+    <t>إجمالي عدد الطلاب</t>
+  </si>
+  <si>
+    <t>TOTAL NUMBER OF STUDENTS</t>
+  </si>
+  <si>
+    <t>OPEN SEATS</t>
+  </si>
+  <si>
+    <t>UTILIZATION RATE</t>
+  </si>
+  <si>
+    <t>MAXIMUM ENROLLMENT CAPACTIY</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>مقاعد مفتوحة</t>
+  </si>
+  <si>
+    <t>معدل الاستخدام</t>
+  </si>
+  <si>
+    <t>الحد الأقصى لسعة التسجيل</t>
+  </si>
+  <si>
+    <t>الوحدات</t>
+  </si>
+  <si>
+    <t>Enrollment</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>التسجيل</t>
+  </si>
+  <si>
+    <t>سعة</t>
+  </si>
+  <si>
+    <t>Number Of Senior Administrators</t>
+  </si>
+  <si>
+    <t>عدد كبار الإداريين</t>
+  </si>
+  <si>
+    <t>Land Size (SQM)</t>
+  </si>
+  <si>
+    <t>مساحة الأرض (متر مربع)</t>
+  </si>
+  <si>
+    <t>TOTAL TEACHERS</t>
+  </si>
+  <si>
+    <t>مجموع المعلمين</t>
+  </si>
+  <si>
+    <t>Forecasts</t>
+  </si>
+  <si>
+    <t>التنبؤات</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -115,6 +529,19 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,7 +564,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -145,6 +572,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,10 +797,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -471,7 +905,600 @@
         <v>23</v>
       </c>
     </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B63" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B64" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B65" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B66" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B69" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B71" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B72" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B73" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B74" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B75" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B76" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B77" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B78" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B79" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B80" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B81" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B82" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B83" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B84" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B86" t="s">
+        <v>161</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>